<commit_message>
add iot proposed plan
</commit_message>
<xml_diff>
--- a/Monitoring.xlsx
+++ b/Monitoring.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aphan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitMe\anphan2410\TextFileTransfer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
     <sheet name="SE team weekly" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="94">
   <si>
     <t>Thang</t>
   </si>
@@ -166,52 +166,192 @@
     <t>Directly Report To</t>
   </si>
   <si>
-    <t>Learn Access</t>
-  </si>
-  <si>
-    <t>go to lyndacourse</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Son</t>
-  </si>
-  <si>
-    <t>Fast Answers to Access problems in future</t>
-  </si>
-  <si>
-    <t>watch time: 18h
-practice time: 18h
-tolerance: 5h</t>
-  </si>
-  <si>
-    <t>41h</t>
-  </si>
-  <si>
-    <t>depend on other tasks</t>
-  </si>
-  <si>
-    <t>not approved
-not started</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Path</t>
-  </si>
-  <si>
-    <t>/AscenX/SETeam/ioTProject/FlipperMonitor/Milestone1</t>
-  </si>
-  <si>
     <t>Up-to-date Actuality</t>
+  </si>
+  <si>
+    <t>piLocalDBWorker</t>
+  </si>
+  <si>
+    <t>a thread that provides write/read functions with local database on pi</t>
+  </si>
+  <si>
+    <t>_Code + Diagram</t>
+  </si>
+  <si>
+    <t>learn and test qsql : 8h
+meeting with team: 3h
+raw state diagram : 5h
+raw code : 5h
+raw test + revise : 5h
+tolerance : 5h</t>
+  </si>
+  <si>
+    <t>Tâm : 3h
+Đăng : 3h
+Đăng code
+Đăng database</t>
+  </si>
+  <si>
+    <t>Tâm</t>
+  </si>
+  <si>
+    <t>31h</t>
+  </si>
+  <si>
+    <t>wait for approval</t>
+  </si>
+  <si>
+    <t>a thread that provides write/read functions with online database VPS2</t>
+  </si>
+  <si>
+    <t>work with Đăng : 8h
+meeting with team : 3h
+raw state diagram : 5h
+raw code : 5h
+raw test + revise : 5h
+tolerance : 5h</t>
+  </si>
+  <si>
+    <t>Tâm : 3h
+Đăng : 11h
+Đăng code</t>
+  </si>
+  <si>
+    <t>Online VPS2 DB Communicator</t>
+  </si>
+  <si>
+    <t>Logger</t>
+  </si>
+  <si>
+    <t>_Code + Example</t>
+  </si>
+  <si>
+    <t>an excel log recording program activities at running time</t>
+  </si>
+  <si>
+    <t>raw flow chart : 8h
+raw code : 8h
+raw test + revise : 5h
+tolerance : 5h</t>
+  </si>
+  <si>
+    <t>_Basic Function: Initialize/Write/Read
+_Code + Diagram</t>
+  </si>
+  <si>
+    <t>_Basic Function: Write/Read
+_Code + Diagram</t>
+  </si>
+  <si>
+    <t>26h</t>
+  </si>
+  <si>
+    <t>Auto UHV2 PVI Collector</t>
+  </si>
+  <si>
+    <t>a thread collecting PVI of UHV2 and put into database</t>
+  </si>
+  <si>
+    <t>raw state diagram : 3h
+raw code : 3h
+raw test + revise : 3h
+tolerance : 5h</t>
+  </si>
+  <si>
+    <t>Auto UHV4 PVI Collector</t>
+  </si>
+  <si>
+    <t>a thread collecting PVI of UHV4 and put into database</t>
+  </si>
+  <si>
+    <t>raw state diagram : 1h
+raw code : 1h
+raw test + revise : 1h
+tolerance : 3h</t>
+  </si>
+  <si>
+    <t>Auto CAN Data Collector</t>
+  </si>
+  <si>
+    <t>a thread collecting RFID and put into database</t>
+  </si>
+  <si>
+    <t>Tâm: 3h</t>
+  </si>
+  <si>
+    <t>meeting with Tâm: 3h
+raw state diagram : 3h
+raw code : 3h
+raw test + revise : 3h
+tolerance : 5h</t>
+  </si>
+  <si>
+    <t>17h</t>
+  </si>
+  <si>
+    <t>5h</t>
+  </si>
+  <si>
+    <t>20h</t>
+  </si>
+  <si>
+    <t>Small Coordinator</t>
+  </si>
+  <si>
+    <t>a thread directing the data</t>
+  </si>
+  <si>
+    <t>meeting with Tâm: 5h
+raw state diagram : 5h
+raw code: 5h
+raw test + revise : 8h
+tolerance: 8h</t>
+  </si>
+  <si>
+    <t>Tâm: 5h</t>
+  </si>
+  <si>
+    <t>Combination</t>
+  </si>
+  <si>
+    <t>refractor and revise code, to make all things work in harmony</t>
+  </si>
+  <si>
+    <t>raw work: 5h
+test + revise : 5h
+tolerance:8h</t>
+  </si>
+  <si>
+    <t>18h</t>
+  </si>
+  <si>
+    <t>Big Test + Fix Bug</t>
+  </si>
+  <si>
+    <t>raw work: 10h
+tolerance: 10h</t>
+  </si>
+  <si>
+    <t>_Code + Accessment</t>
+  </si>
+  <si>
+    <t>all kind of functions will be test</t>
+  </si>
+  <si>
+    <t>199h</t>
+  </si>
+  <si>
+    <t>Tâm : 14h
+Đăng: 14h</t>
+  </si>
+  <si>
+    <t>EDCTU Software</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -320,7 +460,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -482,6 +622,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -489,7 +685,7 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -537,6 +733,24 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="17" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -561,58 +775,61 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -949,38 +1166,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="39" t="s">
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="41" t="s">
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="42"/>
-      <c r="V1" s="42"/>
-      <c r="W1" s="42"/>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="42"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="48"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
@@ -2094,46 +2311,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="46" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" style="46" customWidth="1"/>
-    <col min="3" max="3" width="18" style="46" customWidth="1"/>
-    <col min="4" max="6" width="21.140625" style="46" customWidth="1"/>
-    <col min="7" max="7" width="13" style="46" customWidth="1"/>
-    <col min="8" max="9" width="16.42578125" style="46" customWidth="1"/>
-    <col min="10" max="13" width="16.140625" style="46" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" style="46" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="44"/>
+    <col min="1" max="1" width="19.28515625" style="37" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="37" customWidth="1"/>
+    <col min="3" max="3" width="31" style="37" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="37" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" style="37" customWidth="1"/>
+    <col min="6" max="6" width="13" style="37" customWidth="1"/>
+    <col min="7" max="8" width="16.42578125" style="37" customWidth="1"/>
+    <col min="9" max="12" width="16.140625" style="37" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" style="37" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="45" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:13" s="36" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="50"/>
-    </row>
-    <row r="2" spans="1:14" s="45" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="56"/>
+    </row>
+    <row r="2" spans="1:13" s="36" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="51" t="s">
         <v>35</v>
       </c>
@@ -2141,147 +2358,371 @@
       <c r="C2" s="52"/>
       <c r="D2" s="52"/>
       <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="51" t="s">
+      <c r="F2" s="53"/>
+      <c r="G2" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="51" t="s">
+      <c r="H2" s="52"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="51" t="s">
         <v>35</v>
       </c>
+      <c r="K2" s="52"/>
       <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="53"/>
-    </row>
-    <row r="3" spans="1:14" s="45" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="M2" s="53"/>
+    </row>
+    <row r="3" spans="1:13" s="36" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="59"/>
+      <c r="E3" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="57" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="58"/>
+    </row>
+    <row r="4" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="59"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="50"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="39" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="90.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+    </row>
+    <row r="6" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="55" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="55" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="M3" s="58" t="s">
-        <v>41</v>
-      </c>
-      <c r="N3" s="59"/>
-    </row>
-    <row r="4" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="54" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="57"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="N4" s="54" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="47" t="s">
+      <c r="D6" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" s="47" t="s">
+      <c r="E6" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="60">
-        <v>42919</v>
-      </c>
-      <c r="I5" s="47" t="s">
+      <c r="F7" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="J8" s="38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="47" t="s">
+      <c r="J10" s="38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="K5" s="47" t="s">
+      <c r="I11" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="J11" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="L5" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="N5" s="47" t="s">
-        <v>55</v>
-      </c>
+    </row>
+    <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="63" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+    </row>
+    <row r="14" spans="1:13" s="62" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="66"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" s="66" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" s="66"/>
+      <c r="L14" s="66"/>
+      <c r="M14" s="67"/>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="38"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="16">
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="C3:C4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2302,13 +2743,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>

</xml_diff>